<commit_message>
High Stakes Gambling (GB) - add badges, more dev/testing
</commit_message>
<xml_diff>
--- a/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
+++ b/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2AFDC1-7FB8-4FB8-80F6-1D8FE049958F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFE6F45-41C7-436B-8D5E-D89F385E9636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28485" yWindow="765" windowWidth="28485" windowHeight="15435" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Keep" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
     <sheet name="Testing" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Keep!$A$1:$J$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Keep!$A$1:$I$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Reject!$A$1:$I$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Testing!$A$1:$G$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Testing!$A$1:$G$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="300">
   <si>
     <t>Name</t>
   </si>
@@ -350,9 +350,6 @@
     <t>Progression</t>
   </si>
   <si>
-    <t>Intro</t>
-  </si>
-  <si>
     <t>Item Usage</t>
   </si>
   <si>
@@ -530,9 +527,6 @@
     <t>Sit Up Straight &amp; Don't Forget to Flush</t>
   </si>
   <si>
-    <t>[Competitive/Blackjack] Save time by having your opponent run out of cash before Hand 10 *player doesn't have much control over outcome</t>
-  </si>
-  <si>
     <t>[Competitive/Blackjack] Make your opponent bust with a "very non-suspicious" hand value of 35 points or more</t>
   </si>
   <si>
@@ -611,9 +605,6 @@
     <t>Craps Basics - Mama Told Me Not To</t>
   </si>
   <si>
-    <t>[Practice/Craps] Win a line, multi-roll, and single-roll bet on the same roll without losing any bets that roll</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -707,9 +698,6 @@
     <t>[Practice/Craps] Starting with $10,000, double your money</t>
   </si>
   <si>
-    <t>[Practice/Craps] Win multiple bets at once? (e.g. on a single roll, win at least 5? bets without losing any bets)</t>
-  </si>
-  <si>
     <t>TODO</t>
   </si>
   <si>
@@ -752,9 +740,6 @@
     <t>That's a Lot for the 1930s, Then Adjust For Inflation</t>
   </si>
   <si>
-    <t>[Competitive/Blackjack] Save time by having your opponent run out of cash before Hand 10 *nearly impossible/opponent reduces bet as money gets lower/player doesn't have much control over outcome</t>
-  </si>
-  <si>
     <t>Sounds Like Rain</t>
   </si>
   <si>
@@ -791,9 +776,6 @@
     <t>Craps Basics - Rollin', Rollin', Rollin'</t>
   </si>
   <si>
-    <t>[Practice/Craps] Win a line, multi-roll, and single-roll bet on the same dice roll without losing any bets that roll</t>
-  </si>
-  <si>
     <t>implement</t>
   </si>
   <si>
@@ -833,9 +815,6 @@
     <t>(Blackjack) use Ace or King cheat and get B.J.?</t>
   </si>
   <si>
-    <t>basically just luck</t>
-  </si>
-  <si>
     <t>(Blackjack) swap opponent's Blackjack</t>
   </si>
   <si>
@@ -908,10 +887,58 @@
     <t>false trigger when opponent only bet (not raised) then player won hand (b/c "Player's Last Actual Bet Amount" not cleared from previous hand)</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Badge</t>
+    <t>[Competitive/Any Mission] Accumulate at least $500K total end-of-mission winnings (excludes password-loaded winnings)</t>
+  </si>
+  <si>
+    <t>easy/limit achievement spam</t>
+  </si>
+  <si>
+    <t>[Any Mode/Any Poker] Win hand with Straight (5x payout in Video Poker) or Flush (8x)</t>
+  </si>
+  <si>
+    <t>[Any Mode/Any Poker] Win hand with Full House (20x payout in Video Poker) or 4 of a Kind (50x)</t>
+  </si>
+  <si>
+    <t>[Any Mode/Any Poker] Win hand with Straight Flush (100x payout) or Royal Flush (250x)</t>
+  </si>
+  <si>
+    <t>AnyP</t>
+  </si>
+  <si>
+    <t>[Competitive/Mission 4] Complete Mission 4 with at least 350K in cash winnings</t>
+  </si>
+  <si>
+    <t>[Competitive/Mission 3] Complete Mission 3 in 6 hands or less of Draw Poker</t>
+  </si>
+  <si>
+    <t>Name TBD</t>
+  </si>
+  <si>
+    <t>[Competitive/Blackjack] Save time by having your opponent run out of cash before Hand 10</t>
+  </si>
+  <si>
+    <t>nearly impossible/opponent reduces bet as money gets lower/player has little control over outcome</t>
+  </si>
+  <si>
+    <t>[Competitive/Draw Poker] win without losing a single hand</t>
+  </si>
+  <si>
+    <t>probably considered bad design b/c making player do silly stuff without any in-game effect</t>
+  </si>
+  <si>
+    <t>[Practice/Craps] Bet on every possible bet at once</t>
+  </si>
+  <si>
+    <t>[Practice/Craps] Have exactly 9 bets on the table and win them all on the same roll</t>
+  </si>
+  <si>
+    <t>[Practice/Craps] Win a line, multi-roll, and single-roll bet on the same roll (without any other bets on the table)</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>just luck/no challenge</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1003,9 +1030,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1389,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7279781E-0A72-4F8F-8555-23E2F15EEC5A}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,12 +1431,11 @@
     <col min="7" max="7" width="68" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1424,10 +1447,10 @@
         <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1438,11 +1461,8 @@
       <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1450,16 +1470,16 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1468,7 +1488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1476,16 +1496,16 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" t="s">
         <v>61</v>
@@ -1497,7 +1517,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1505,16 +1525,16 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
         <v>38</v>
@@ -1523,10 +1543,10 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1534,16 +1554,16 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1552,7 +1572,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1560,13 +1580,13 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
@@ -1575,13 +1595,10 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>214</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1589,13 +1606,13 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -1607,10 +1624,10 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1618,16 +1635,16 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1636,7 +1653,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1644,25 +1661,25 @@
         <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1670,16 +1687,16 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
         <v>102</v>
       </c>
       <c r="E10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" t="s">
         <v>112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>113</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -1687,25 +1704,22 @@
       <c r="I10" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
         <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
@@ -1716,11 +1730,8 @@
       <c r="I11" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1728,16 +1739,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
         <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -1745,11 +1756,8 @@
       <c r="I12" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1757,16 +1765,16 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" t="s">
         <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -1774,11 +1782,8 @@
       <c r="I13" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1786,16 +1791,16 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
         <v>102</v>
       </c>
       <c r="E14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" t="s">
         <v>112</v>
-      </c>
-      <c r="F14" t="s">
-        <v>113</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -1803,11 +1808,8 @@
       <c r="I14" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1815,13 +1817,13 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
         <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
         <v>51</v>
@@ -1832,11 +1834,8 @@
       <c r="I15" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1844,16 +1843,16 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H16">
         <v>3</v>
@@ -1861,11 +1860,8 @@
       <c r="I16" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1873,16 +1869,16 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
         <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -1890,11 +1886,8 @@
       <c r="I17" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1902,16 +1895,16 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
         <v>102</v>
       </c>
       <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" t="s">
         <v>112</v>
-      </c>
-      <c r="F18" t="s">
-        <v>113</v>
       </c>
       <c r="H18">
         <v>4</v>
@@ -1919,11 +1912,8 @@
       <c r="I18" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1931,13 +1921,13 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
         <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
@@ -1948,11 +1938,8 @@
       <c r="I19" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1960,16 +1947,16 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
         <v>102</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
         <v>35</v>
@@ -1980,11 +1967,8 @@
       <c r="I20" t="s">
         <v>90</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1992,16 +1976,16 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
         <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -2009,11 +1993,8 @@
       <c r="I21" t="s">
         <v>90</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2021,16 +2002,16 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" t="s">
         <v>102</v>
       </c>
       <c r="E22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" t="s">
         <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>113</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -2038,11 +2019,8 @@
       <c r="I22" t="s">
         <v>90</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2050,13 +2028,13 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" t="s">
         <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
         <v>51</v>
@@ -2067,11 +2045,8 @@
       <c r="I23" t="s">
         <v>90</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2079,16 +2054,16 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
         <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -2096,11 +2071,8 @@
       <c r="I24" t="s">
         <v>90</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2108,16 +2080,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" t="s">
         <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -2125,11 +2097,8 @@
       <c r="I25" t="s">
         <v>90</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2137,16 +2106,16 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
         <v>102</v>
       </c>
       <c r="E26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" t="s">
         <v>112</v>
-      </c>
-      <c r="F26" t="s">
-        <v>113</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -2154,11 +2123,8 @@
       <c r="I26" t="s">
         <v>90</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2166,19 +2132,19 @@
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27" t="s">
         <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
         <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H27">
         <v>5</v>
@@ -2186,28 +2152,25 @@
       <c r="I27" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
         <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" t="s">
         <v>36</v>
@@ -2218,11 +2181,8 @@
       <c r="I28" t="s">
         <v>90</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2230,19 +2190,19 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
         <v>102</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -2250,11 +2210,8 @@
       <c r="I29" t="s">
         <v>90</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2262,16 +2219,16 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
         <v>102</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H30">
         <v>25</v>
@@ -2279,11 +2236,8 @@
       <c r="I30" t="s">
         <v>90</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2291,25 +2245,25 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" t="s">
         <v>112</v>
-      </c>
-      <c r="F31" t="s">
-        <v>113</v>
       </c>
       <c r="H31">
         <v>5</v>
       </c>
       <c r="I31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2317,25 +2271,25 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" t="s">
         <v>112</v>
-      </c>
-      <c r="F32" t="s">
-        <v>113</v>
       </c>
       <c r="H32">
         <v>5</v>
       </c>
       <c r="I32" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2343,16 +2297,16 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" t="s">
         <v>112</v>
-      </c>
-      <c r="F33" t="s">
-        <v>113</v>
       </c>
       <c r="H33">
         <v>3</v>
@@ -2361,7 +2315,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2369,16 +2323,16 @@
         <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" t="s">
         <v>112</v>
-      </c>
-      <c r="F34" t="s">
-        <v>113</v>
       </c>
       <c r="G34" t="s">
         <v>43</v>
@@ -2390,21 +2344,21 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F35" t="s">
         <v>51</v>
@@ -2416,7 +2370,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2424,16 +2378,16 @@
         <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" t="s">
         <v>85</v>
@@ -2442,10 +2396,10 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2453,39 +2407,39 @@
         <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F38" t="s">
         <v>51</v>
@@ -2494,10 +2448,10 @@
         <v>5</v>
       </c>
       <c r="I38" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2505,13 +2459,13 @@
         <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39" t="s">
         <v>51</v>
@@ -2523,13 +2477,10 @@
         <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>214</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2537,13 +2488,13 @@
         <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F40" t="s">
         <v>51</v>
@@ -2552,13 +2503,10 @@
         <v>4</v>
       </c>
       <c r="I40" t="s">
-        <v>214</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2566,13 +2514,13 @@
         <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" t="s">
         <v>51</v>
@@ -2581,13 +2529,10 @@
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>214</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2595,13 +2540,13 @@
         <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F42" t="s">
         <v>51</v>
@@ -2613,13 +2558,10 @@
         <v>25</v>
       </c>
       <c r="I42" t="s">
-        <v>214</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2627,94 +2569,94 @@
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H43">
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>284</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F44" t="s">
-        <v>115</v>
+        <v>287</v>
       </c>
       <c r="H44">
         <v>4</v>
       </c>
       <c r="I44" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>285</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
-        <v>115</v>
+        <v>287</v>
       </c>
       <c r="H45">
         <v>5</v>
       </c>
       <c r="I45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>286</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" t="s">
-        <v>114</v>
+        <v>287</v>
       </c>
       <c r="G46" t="s">
         <v>84</v>
@@ -2723,36 +2665,36 @@
         <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H47">
         <v>10</v>
       </c>
       <c r="I47" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2760,16 +2702,16 @@
         <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H48">
         <v>5</v>
@@ -2778,7 +2720,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2786,42 +2728,42 @@
         <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H49">
         <v>5</v>
       </c>
       <c r="I49" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C50" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D50" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G50" t="s">
         <v>87</v>
@@ -2830,30 +2772,30 @@
         <v>10</v>
       </c>
       <c r="I50" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C51" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D51" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F51" t="s">
         <v>51</v>
       </c>
       <c r="G51" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H51">
         <v>3</v>
@@ -2862,7 +2804,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2870,19 +2812,19 @@
         <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H52">
         <v>10</v>
@@ -2890,40 +2832,34 @@
       <c r="I52" t="s">
         <v>90</v>
       </c>
-      <c r="J52" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C53" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H53">
         <v>25</v>
       </c>
       <c r="I53" t="s">
-        <v>214</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2931,16 +2867,16 @@
         <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H54">
         <v>10</v>
@@ -2949,7 +2885,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2957,16 +2893,16 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" t="s">
         <v>112</v>
-      </c>
-      <c r="F55" t="s">
-        <v>113</v>
       </c>
       <c r="H55">
         <v>10</v>
@@ -2975,7 +2911,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2983,91 +2919,91 @@
         <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E56" t="s">
+        <v>111</v>
+      </c>
+      <c r="F56" t="s">
         <v>112</v>
-      </c>
-      <c r="F56" t="s">
-        <v>113</v>
       </c>
       <c r="H56">
         <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="D57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H57">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H58">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
       <c r="D59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F59" t="s">
         <v>115</v>
@@ -3076,27 +3012,27 @@
         <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H60">
         <v>10</v>
@@ -3105,79 +3041,76 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>290</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>288</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F61" t="s">
-        <v>116</v>
-      </c>
-      <c r="G61" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="H61">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I61" t="s">
         <v>90</v>
       </c>
-      <c r="J61" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="D62" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E62" t="s">
         <v>111</v>
       </c>
       <c r="F62" t="s">
-        <v>82</v>
+        <v>115</v>
+      </c>
+      <c r="G62" t="s">
+        <v>28</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I62" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D63" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F63" t="s">
         <v>82</v>
@@ -3189,27 +3122,24 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C64" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F64" t="s">
         <v>82</v>
-      </c>
-      <c r="G64" t="s">
-        <v>187</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3223,22 +3153,22 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="C65" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F65" t="s">
         <v>82</v>
       </c>
       <c r="G65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -3252,19 +3182,22 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C66" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D66" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F66" t="s">
         <v>82</v>
+      </c>
+      <c r="G66" t="s">
+        <v>186</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -3278,22 +3211,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C67" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D67" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F67" t="s">
         <v>82</v>
-      </c>
-      <c r="G67" t="s">
-        <v>186</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -3307,22 +3237,25 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>248</v>
+        <v>183</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
       <c r="D68" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F68" t="s">
         <v>82</v>
       </c>
+      <c r="G68" t="s">
+        <v>184</v>
+      </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68" t="s">
         <v>90</v>
@@ -3333,16 +3266,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D69" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="E69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F69" t="s">
         <v>82</v>
@@ -3359,25 +3292,25 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>244</v>
+      </c>
+      <c r="C70" t="s">
         <v>180</v>
       </c>
-      <c r="C70" t="s">
-        <v>250</v>
-      </c>
       <c r="D70" t="s">
-        <v>105</v>
+        <v>298</v>
       </c>
       <c r="E70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F70" t="s">
         <v>82</v>
       </c>
       <c r="H70">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I70" t="s">
-        <v>214</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3385,16 +3318,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
       <c r="C71" t="s">
-        <v>222</v>
+        <v>297</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F71" t="s">
         <v>82</v>
@@ -3403,7 +3336,7 @@
         <v>5</v>
       </c>
       <c r="I71" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3411,16 +3344,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>296</v>
       </c>
       <c r="D72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F72" t="s">
         <v>82</v>
@@ -3429,11 +3362,37 @@
         <v>10</v>
       </c>
       <c r="I72" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" t="s">
+        <v>105</v>
+      </c>
+      <c r="E73" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73" t="s">
+        <v>82</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J72" xr:uid="{7279781E-0A72-4F8F-8555-23E2F15EEC5A}"/>
+  <autoFilter ref="A1:I73" xr:uid="{7279781E-0A72-4F8F-8555-23E2F15EEC5A}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3442,11 +3401,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334CAE3C-4AD9-46C5-82BD-40A7611E1FF0}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,10 +3432,10 @@
         <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -3485,10 +3444,10 @@
         <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3496,16 +3455,16 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3514,7 +3473,7 @@
         <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3525,13 +3484,13 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3540,7 +3499,7 @@
         <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3551,10 +3510,10 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -3566,7 +3525,7 @@
         <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3577,13 +3536,13 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -3592,7 +3551,7 @@
         <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3603,10 +3562,10 @@
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
         <v>82</v>
@@ -3618,7 +3577,7 @@
         <v>92</v>
       </c>
       <c r="I6" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3626,16 +3585,16 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s">
         <v>62</v>
@@ -3647,7 +3606,7 @@
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3655,16 +3614,16 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
         <v>112</v>
-      </c>
-      <c r="E8" t="s">
-        <v>113</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -3673,7 +3632,7 @@
         <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3681,16 +3640,16 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="s">
         <v>112</v>
-      </c>
-      <c r="E9" t="s">
-        <v>113</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -3699,7 +3658,7 @@
         <v>92</v>
       </c>
       <c r="I9" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3710,10 +3669,10 @@
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -3730,16 +3689,16 @@
         <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
         <v>55</v>
@@ -3751,7 +3710,7 @@
         <v>92</v>
       </c>
       <c r="I11" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3762,13 +3721,13 @@
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -3777,7 +3736,7 @@
         <v>92</v>
       </c>
       <c r="I12" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3788,13 +3747,13 @@
         <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
         <v>68</v>
@@ -3806,7 +3765,7 @@
         <v>92</v>
       </c>
       <c r="I13" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3817,13 +3776,13 @@
         <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -3832,7 +3791,7 @@
         <v>92</v>
       </c>
       <c r="I14" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3843,13 +3802,13 @@
         <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -3861,7 +3820,7 @@
         <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3872,13 +3831,13 @@
         <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" t="s">
         <v>73</v>
@@ -3890,7 +3849,7 @@
         <v>92</v>
       </c>
       <c r="I16" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3898,16 +3857,16 @@
         <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>99</v>
@@ -3916,7 +3875,7 @@
         <v>92</v>
       </c>
       <c r="I17" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3924,13 +3883,13 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
@@ -3947,16 +3906,16 @@
         <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
         <v>85</v>
@@ -3970,16 +3929,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" t="s">
         <v>92</v>
@@ -3987,13 +3946,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" t="s">
         <v>82</v>
@@ -4005,7 +3964,7 @@
         <v>92</v>
       </c>
       <c r="I21" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4013,16 +3972,16 @@
         <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" t="s">
         <v>28</v>
@@ -4034,27 +3993,27 @@
         <v>90</v>
       </c>
       <c r="I22" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G23">
         <v>25</v>
@@ -4063,27 +4022,27 @@
         <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
         <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -4092,24 +4051,24 @@
         <v>92</v>
       </c>
       <c r="I24" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G25">
         <v>25</v>
@@ -4118,7 +4077,79 @@
         <v>92</v>
       </c>
       <c r="I25" t="s">
-        <v>276</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>295</v>
+      </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -4133,7 +4164,7 @@
   <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,22 +4181,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -4177,18 +4208,18 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
       <c r="F3">
         <f>COUNTIF(Keep!D:D,"="&amp;E3)</f>
         <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K3">
         <f>COUNT(Keep!H:H)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -4207,11 +4238,11 @@
         <v>21</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K4">
         <f>SUM(Keep!H:H)</f>
-        <v>429</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -4223,14 +4254,14 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F5">
         <f>SUM(H5:H7)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5">
         <f>COUNTIF(Keep!D:D,"="&amp;G5)</f>
@@ -4246,18 +4277,18 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6">
         <f>COUNTIF(Keep!D:D,"="&amp;G6)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K6">
         <f>COUNTIFS(Testing!C:C,"=Yes",Testing!D:D,"&lt;&gt;Yes")</f>
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -4266,17 +4297,17 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Keep!H:H,"="&amp;B7)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H7">
         <f>COUNTIF(Keep!D:D,"="&amp;G7)</f>
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K7">
         <f>COUNTIF(Testing!C:C,"=No") + COUNTIF(Testing!C:C,"=No (retest)") + COUNTIF(Testing!D:D,"=Yes") - COUNTIFS(Testing!C:C,"=No",Testing!D:D,"=Yes") - COUNTIFS(Testing!C:C,"=No (retest)",Testing!D:D,"=Yes")</f>
@@ -4289,21 +4320,21 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Keep!H:H,"="&amp;B8)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8">
         <f>COUNTIF(Keep!D:D,"="&amp;E8)</f>
         <v>3</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K8">
         <f>K3-K6-K7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -4315,11 +4346,11 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9">
         <f>COUNTIF(Keep!D:D,"="&amp;E9)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -4342,15 +4373,15 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13">
         <f>COUNTIF(Keep!F:F,"="&amp;E13)</f>
@@ -4368,20 +4399,20 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15">
         <f>COUNTIF(Keep!F:F,"="&amp;E15)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16">
         <f>COUNTIF(Keep!F:F,"="&amp;E16)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
@@ -4395,20 +4426,20 @@
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>117</v>
+        <v>287</v>
       </c>
       <c r="F18">
         <f>COUNTIF(Keep!F:F,"="&amp;E18)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F19">
         <f>COUNTIF(Keep!F:F,"="&amp;E19)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4424,11 +4455,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4217636D-3F58-4C31-B7F4-A1FB83661293}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4450,24 +4481,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4475,7 +4506,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
@@ -4489,7 +4520,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
         <v>90</v>
@@ -4503,7 +4534,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
         <v>90</v>
@@ -4517,7 +4548,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>90</v>
@@ -4531,7 +4562,7 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
         <v>90</v>
@@ -4545,7 +4576,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
         <v>90</v>
@@ -4559,7 +4590,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
         <v>90</v>
@@ -4573,7 +4604,7 @@
         <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>90</v>
@@ -4592,7 +4623,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>90</v>
@@ -4603,10 +4634,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>90</v>
@@ -4620,7 +4651,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
         <v>90</v>
@@ -4634,7 +4665,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
@@ -4648,7 +4679,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
         <v>90</v>
@@ -4662,7 +4693,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
         <v>90</v>
@@ -4676,7 +4707,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -4690,7 +4721,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
         <v>90</v>
@@ -4704,7 +4735,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
@@ -4718,7 +4749,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
         <v>90</v>
@@ -4732,7 +4763,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
@@ -4746,7 +4777,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
         <v>90</v>
@@ -4757,10 +4788,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
         <v>90</v>
@@ -4774,7 +4805,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
         <v>90</v>
@@ -4788,7 +4819,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
         <v>90</v>
@@ -4802,7 +4833,7 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
         <v>90</v>
@@ -4816,7 +4847,7 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s">
         <v>90</v>
@@ -4830,7 +4861,7 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
         <v>90</v>
@@ -4841,10 +4872,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" t="s">
         <v>90</v>
@@ -4858,7 +4889,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
         <v>90</v>
@@ -4872,7 +4903,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
         <v>90</v>
@@ -4883,7 +4914,7 @@
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4891,13 +4922,13 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
         <v>90</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4905,7 +4936,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
         <v>90</v>
@@ -4916,7 +4947,7 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
         <v>90</v>
@@ -4927,7 +4958,7 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -4935,10 +4966,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
         <v>90</v>
@@ -4949,13 +4980,13 @@
         <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
         <v>90</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4963,7 +4994,7 @@
         <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C40" t="s">
         <v>90</v>
@@ -4972,23 +5003,23 @@
         <v>90</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C42" t="s">
         <v>90</v>
@@ -4999,7 +5030,7 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
         <v>90</v>
@@ -5010,7 +5041,7 @@
         <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
@@ -5021,7 +5052,7 @@
         <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
@@ -5032,7 +5063,7 @@
         <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
         <v>90</v>
@@ -5043,7 +5074,7 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
         <v>90</v>
@@ -5051,96 +5082,96 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>159</v>
       </c>
-      <c r="B49" t="s">
-        <v>167</v>
-      </c>
-      <c r="C49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>161</v>
-      </c>
-      <c r="B50" t="s">
-        <v>166</v>
-      </c>
-      <c r="C50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>160</v>
-      </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C54" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>205</v>
+      </c>
+      <c r="B55" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>208</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>209</v>
       </c>
-      <c r="C55" t="s">
-        <v>90</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>211</v>
-      </c>
-      <c r="B56" t="s">
-        <v>212</v>
-      </c>
       <c r="C56" t="s">
         <v>90</v>
       </c>
@@ -5148,80 +5179,86 @@
         <v>90</v>
       </c>
       <c r="F56" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B59" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C59" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" t="s">
-        <v>280</v>
-      </c>
-      <c r="C60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>235</v>
       </c>
       <c r="C62" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
-        <v>240</v>
-      </c>
-      <c r="C63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>163</v>
+        <v>293</v>
       </c>
       <c r="C64" t="s">
         <v>90</v>
@@ -5229,27 +5266,27 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D65" t="s">
-        <v>90</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>288</v>
+        <v>272</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E65" t="s">
+        <v>90</v>
+      </c>
+      <c r="G65" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="C66" t="s">
         <v>90</v>
@@ -5257,54 +5294,42 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>279</v>
-      </c>
-      <c r="C67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E67" t="s">
-        <v>90</v>
-      </c>
-      <c r="G67" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>290</v>
+      </c>
+      <c r="B68" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>22</v>
       </c>
-      <c r="B68" t="s">
-        <v>199</v>
-      </c>
-      <c r="C68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="B69" t="s">
+        <v>196</v>
+      </c>
+      <c r="C69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>179</v>
-      </c>
-      <c r="B70" t="s">
-        <v>241</v>
-      </c>
-      <c r="C70" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
       <c r="C71" t="s">
         <v>90</v>
@@ -5312,10 +5337,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B72" t="s">
-        <v>243</v>
+        <v>276</v>
       </c>
       <c r="C72" t="s">
         <v>90</v>
@@ -5323,10 +5348,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B73" t="s">
-        <v>284</v>
+        <v>238</v>
       </c>
       <c r="C73" t="s">
         <v>90</v>
@@ -5334,10 +5359,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B74" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="C74" t="s">
         <v>90</v>
@@ -5345,10 +5370,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C75" t="s">
         <v>90</v>
@@ -5356,55 +5381,49 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>253</v>
+        <v>241</v>
+      </c>
+      <c r="C76" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77" t="s">
-        <v>90</v>
+        <v>181</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>244</v>
+      </c>
+      <c r="B78" t="s">
         <v>180</v>
       </c>
-      <c r="B78" t="s">
-        <v>190</v>
-      </c>
       <c r="C78" t="s">
         <v>90</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>251</v>
+      <c r="G78" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>297</v>
       </c>
       <c r="C79" t="s">
         <v>90</v>
@@ -5413,22 +5432,39 @@
         <v>90</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>221</v>
+        <v>296</v>
       </c>
       <c r="C80" t="s">
         <v>90</v>
       </c>
+      <c r="D80" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G80" xr:uid="{4217636D-3F58-4C31-B7F4-A1FB83661293}"/>
+  <autoFilter ref="A1:G81" xr:uid="{4217636D-3F58-4C31-B7F4-A1FB83661293}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
High Stakes Gambling (GB) - measured flags, point adjustments, minor cleanup
</commit_message>
<xml_diff>
--- a/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
+++ b/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE03C0EB-4066-475F-AA75-0BE73C55E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1F64D-9320-48C7-9390-8FDB3BB8C9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="180" windowWidth="28485" windowHeight="15435" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
+    <workbookView xWindow="-28485" yWindow="765" windowWidth="28485" windowHeight="15435" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Keep" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1026,7 +1026,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,11 +1410,11 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1706,7 @@
         <v>251</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" t="s">
         <v>80</v>
@@ -1739,7 +1738,7 @@
         <v>41</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" t="s">
         <v>80</v>
@@ -1771,7 +1770,7 @@
         <v>100</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
         <v>80</v>
@@ -2492,7 +2491,7 @@
       <c r="J32" t="s">
         <v>80</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="O32" t="s">
         <v>297</v>
       </c>
     </row>
@@ -3028,7 +3027,7 @@
         <v>99</v>
       </c>
       <c r="H49">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I49" t="s">
         <v>80</v>
@@ -4707,7 +4706,7 @@
       </c>
       <c r="C4">
         <f>COUNTIF(Keep!H:H,"="&amp;B4)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>89</v>
@@ -4721,7 +4720,7 @@
       </c>
       <c r="K4">
         <f>SUM(Keep!H:H)</f>
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -4730,7 +4729,7 @@
       </c>
       <c r="C5">
         <f>COUNTIF(Keep!H:H,"="&amp;B5)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>128</v>
@@ -4776,7 +4775,7 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Keep!H:H,"="&amp;B7)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
         <v>129</v>
@@ -4799,7 +4798,7 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Keep!H:H,"="&amp;B8)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
High Stakes Gambling (GB) - bug fix/optimization
</commit_message>
<xml_diff>
--- a/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
+++ b/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1F64D-9320-48C7-9390-8FDB3BB8C9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559F231-689E-483C-AC76-CF5B4D9AE04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28485" yWindow="765" windowWidth="28485" windowHeight="15435" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -834,18 +834,12 @@
     <t>Other Issue?</t>
   </si>
   <si>
-    <t>test if this can be done without PauseLock</t>
-  </si>
-  <si>
     <t>test if this can be done without PauseLock (start condition + Reset), add Trigger?</t>
   </si>
   <si>
     <t>Slots - Purchase a bonus item (on Spin 3 or 7), place it (with the D-pad), and win the line</t>
   </si>
   <si>
-    <t>needs reworking b/c strat is just bet everywhere, fixed: Any Craps (bet not removed on win) not counted</t>
-  </si>
-  <si>
     <t>[Practice] Video Poker - Hold at least one card and get a higher-scoring hand on the 2nd draw (one pair doesn't score unless Jacks or better)</t>
   </si>
   <si>
@@ -930,10 +924,6 @@
     <t>Video Poker - Have at least 3 Joker cards at the end of the hand (Competitive Mode only)</t>
   </si>
   <si>
-    <t>false trigger when opponent is doing Swap Card evaluation if there are 3+ jokers total (fixed by checking at end of hand)
-triggered when played 2nd joker (opponent had 1 joker as well) - unable to reproduce</t>
-  </si>
-  <si>
     <t>merged into Ready to Take a Stand</t>
   </si>
   <si>
@@ -956,6 +946,13 @@
   </si>
   <si>
     <t>unable to get working (false trigger b/c "Player's Last Actual Bet Amount" isn't cleared from previous hand/draw)</t>
+  </si>
+  <si>
+    <t>(fixed by checking at end of hand) false trigger when opponent is doing Swap Card evaluation if there are 3+ jokers total
+(unable to reproduce) triggered when played 2nd joker (opponent had 1 joker as well)</t>
+  </si>
+  <si>
+    <t>needs reworking b/c strat is just bet everywhere, (fixed) Any Craps (bet not removed on win) not counted</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1026,6 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1414,7 +1412,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C2" t="s">
         <v>236</v>
@@ -1519,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
         <v>239</v>
@@ -1554,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C4" t="s">
         <v>237</v>
@@ -1586,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
         <v>238</v>
@@ -1604,7 +1602,7 @@
         <v>29</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
         <v>136</v>
@@ -1621,10 +1619,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D6" t="s">
         <v>182</v>
@@ -1656,10 +1654,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D7" t="s">
         <v>182</v>
@@ -1688,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
         <v>200</v>
@@ -2369,19 +2367,16 @@
       <c r="M28" t="s">
         <v>80</v>
       </c>
-      <c r="N28" t="s">
-        <v>265</v>
-      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C29" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
         <v>90</v>
@@ -2439,7 +2434,7 @@
         <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D31" t="s">
         <v>90</v>
@@ -2468,7 +2463,7 @@
         <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
@@ -2491,8 +2486,8 @@
       <c r="J32" t="s">
         <v>80</v>
       </c>
-      <c r="O32" t="s">
-        <v>297</v>
+      <c r="O32" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2911,7 +2906,7 @@
         <v>80</v>
       </c>
       <c r="N45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -2922,7 +2917,7 @@
         <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D46" t="s">
         <v>93</v>
@@ -3262,7 +3257,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C57" t="s">
         <v>223</v>
@@ -3291,7 +3286,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C58" t="s">
         <v>231</v>
@@ -3320,7 +3315,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C59" t="s">
         <v>232</v>
@@ -3335,7 +3330,7 @@
         <v>72</v>
       </c>
       <c r="G59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -3352,7 +3347,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C60" t="s">
         <v>233</v>
@@ -3384,10 +3379,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C61" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D61" t="s">
         <v>182</v>
@@ -3413,10 +3408,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C62" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D62" t="s">
         <v>182</v>
@@ -3445,10 +3440,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C63" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D63" t="s">
         <v>182</v>
@@ -3469,7 +3464,7 @@
         <v>80</v>
       </c>
       <c r="O63" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -3477,10 +3472,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C64" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D64" t="s">
         <v>182</v>
@@ -4520,12 +4515,12 @@
         <v>80</v>
       </c>
       <c r="I34" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B35" t="s">
         <v>186</v>
@@ -4546,7 +4541,7 @@
         <v>80</v>
       </c>
       <c r="I35" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4572,7 +4567,7 @@
         <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4601,7 +4596,7 @@
         <v>80</v>
       </c>
       <c r="I37" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4627,7 +4622,7 @@
         <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4683,7 +4678,7 @@
       </c>
       <c r="C3">
         <f>COUNTIF(Keep!H:H,"="&amp;B3)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>182</v>
@@ -4706,7 +4701,7 @@
       </c>
       <c r="C4">
         <f>COUNTIF(Keep!H:H,"="&amp;B4)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>89</v>
@@ -4720,7 +4715,7 @@
       </c>
       <c r="K4">
         <f>SUM(Keep!H:H)</f>
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -4831,7 +4826,7 @@
         <v>11</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="K9">
         <f>COUNTIF(Reject!H:H,"=Yes")</f>
@@ -4856,7 +4851,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K11">
         <v>66</v>
@@ -4870,7 +4865,7 @@
         <v>120</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K12">
         <v>11</v>
@@ -4885,7 +4880,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
High Stakes Gambling (GB) - adjust points
</commit_message>
<xml_diff>
--- a/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
+++ b/WIP/High Stakes Gambling (Game Boy)/Docs/achievement_plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559F231-689E-483C-AC76-CF5B4D9AE04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB585B6-C629-4514-83AB-4BB39A31ADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28485" yWindow="765" windowWidth="28485" windowHeight="15435" xr2:uid="{31BE8862-275F-4D32-B8EC-607D115D47ED}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1023,7 +1023,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1412,7 +1411,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,7 +2485,7 @@
       <c r="J32" t="s">
         <v>80</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="O32" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2833,7 +2832,7 @@
         <v>101</v>
       </c>
       <c r="H43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I43" t="s">
         <v>80</v>
@@ -2862,7 +2861,7 @@
         <v>101</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I44" t="s">
         <v>136</v>
@@ -4715,7 +4714,7 @@
       </c>
       <c r="K4">
         <f>SUM(Keep!H:H)</f>
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -4724,7 +4723,7 @@
       </c>
       <c r="C5">
         <f>COUNTIF(Keep!H:H,"="&amp;B5)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>128</v>
@@ -4747,7 +4746,7 @@
       </c>
       <c r="C6">
         <f>COUNTIF(Keep!H:H,"="&amp;B6)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
         <v>91</v>

</xml_diff>